<commit_message>
Projeto finalizado no jupyter!
</commit_message>
<xml_diff>
--- a/MedicoesProjeto.xlsx
+++ b/MedicoesProjeto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/58b32cbac7659b37/Documentos/AULAS_QUARTO_SEMESTRE/Eletromag/Projeto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu.sharepoint.com/sites/LINGLING_40HOURS/Shared Documents/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{640ED4A2-CF60-4FC4-A26B-CE703006E2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{179C0C24-23E8-4B59-AA70-CDBE6B316E70}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{640ED4A2-CF60-4FC4-A26B-CE703006E2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6451AE2-0160-4129-B275-9CCE8489188E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{11381960-7118-4B3E-A32B-235AB83F5534}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{11381960-7118-4B3E-A32B-235AB83F5534}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
-  <si>
-    <t>Para quando a tensão de entrada era de 5V</t>
-  </si>
-  <si>
-    <t>Para quando a tensão de entrada foi 15V</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Potência em Watts</t>
   </si>
@@ -56,12 +50,24 @@
   <si>
     <t>Distância de transmissão [cm]</t>
   </si>
+  <si>
+    <t>ENTRADA DE 5V</t>
+  </si>
+  <si>
+    <t>Potência (W)</t>
+  </si>
+  <si>
+    <t>Potência por distância [W*cm]</t>
+  </si>
+  <si>
+    <t>ENTRADA DE 15V</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,16 +75,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -86,13 +120,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,159 +467,159 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <f>(3.02/2)</f>
         <v>1.51</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>100</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <f>(A3/SQRT(2))^2/100</f>
         <v>1.1400499999999997E-2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <f>C3*B3</f>
         <v>1.1400499999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <f>(5.27/2)</f>
         <v>2.6349999999999998</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>80</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <f t="shared" ref="C4:C7" si="0">(A4/SQRT(2))^2/100</f>
         <v>3.4716124999999994E-2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <f>C4*B4</f>
         <v>2.7772899999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <f>(10.7)/2</f>
         <v>5.35</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>60</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <f t="shared" si="0"/>
         <v>0.14311249999999998</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <f>C5*B5</f>
         <v>8.5867499999999986</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <f>(20.1/2)</f>
         <v>10.050000000000001</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>40</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <f t="shared" si="0"/>
         <v>0.50501250000000009</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <f>C6*B6</f>
         <v>20.200500000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <f>(26.9)/2</f>
         <v>13.45</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>33</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <f t="shared" si="0"/>
         <v>0.90451249999999983</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <f>C7*B7</f>
         <v>29.848912499999994</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <f>82/2</f>
         <v>41</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>33</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <f>(A11/SQRT(2))^2/100</f>
         <v>8.4049999999999994</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <f>C11*B11</f>
         <v>277.36499999999995</v>
       </c>
@@ -574,4 +631,251 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB8BEDFDFEF8EE4EB1C6DE0A0D7E6DDC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b7306b1853557dd0b442b10c6d04d7fb">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4b19d8d-1ea3-402f-b24e-9a143b535671" xmlns:ns3="94498b80-ecb1-43f1-9581-3c977e6898e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8de9ec6f4d0cd4fa40c74e79cdda9db7" ns2:_="" ns3:_="">
+    <xsd:import namespace="a4b19d8d-1ea3-402f-b24e-9a143b535671"/>
+    <xsd:import namespace="94498b80-ecb1-43f1-9581-3c977e6898e2"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a4b19d8d-1ea3-402f-b24e-9a143b535671" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="17" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="94498b80-ecb1-43f1-9581-3c977e6898e2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B837018F-5D14-4492-83C1-0E4F701B5F5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="94498b80-ecb1-43f1-9581-3c977e6898e2"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a4b19d8d-1ea3-402f-b24e-9a143b535671"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D16E0C66-49F9-4F1B-B38D-22AB031C6898}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC10166-0D9A-4CBA-888F-CF72A85A2885}"/>
 </file>
</xml_diff>